<commit_message>
new docs and graphs
</commit_message>
<xml_diff>
--- a/Lit review.xlsx
+++ b/Lit review.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitra\Git\SENG-607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A27710F-0E99-4389-9E8B-D390AE79F687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068D79DA-0626-4779-8DDF-31A1E4C03C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80A05C58-CC51-43DB-AFAF-9143DFD41D5A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{80A05C58-CC51-43DB-AFAF-9143DFD41D5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>link</t>
   </si>
@@ -102,13 +103,83 @@
   </si>
   <si>
     <t>how familiar they are</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP-ON: Prediction of Process Using One-Way Language Model Based on NLP Approach
+</t>
+  </si>
+  <si>
+    <t> text retrieval system, process mining, competator analysis, predictive language models, predictive nlp</t>
+  </si>
+  <si>
+    <t>Novel Use of Natural Language Processing (NLP) to Predict Suicidal Ideation and Psychiatric Symptoms in a Text-Based Mental Health Intervention in Madrid</t>
+  </si>
+  <si>
+    <t>predictive</t>
+  </si>
+  <si>
+    <t>The Use of Word Lists in Textual Analysis</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/15427560.2015.1000335</t>
+  </si>
+  <si>
+    <t>Using Annual Report Sentiment as a Proxy for Financial Distress in U.S. Banks</t>
+  </si>
+  <si>
+    <t>financial - sentiment analysis</t>
+  </si>
+  <si>
+    <t>Intelligent Portfolio Management via NLP Analysis of Financial 10-k Statements</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10796-022-10294-1</t>
+  </si>
+  <si>
+    <t>Implementing Artificial Intelligence in Traditional B2B Marketing Practices: An Activity Theory Perspective</t>
+  </si>
+  <si>
+    <t>https://www.diva-portal.org/smash/get/diva2:833667/FULLTEXT01.pdf</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/11740674_1</t>
+  </si>
+  <si>
+    <t>Using Activity Theory to Model Context Awareness</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/5633674</t>
+  </si>
+  <si>
+    <t>Information Enrichment for Decision Support in Virtual Collaboration</t>
+  </si>
+  <si>
+    <t>Context-aware decision support in knowledge-intensive collaborative e-Work</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1877050910002577</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jamia/article-abstract/17/5/507/830823</t>
+  </si>
+  <si>
+    <t>Mayo clinical Text Analysis and Knowledge Extraction System (cTAKES): architecture, component evaluation and applications </t>
+  </si>
+  <si>
+    <t>A Systematic Review of Natural Language Processing in Healthcare</t>
+  </si>
+  <si>
+    <t>systematic reviews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +210,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF505050"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Merriweather"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -171,6 +254,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -487,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B65E278-8421-40EA-8982-F665D77741A1}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="92.5546875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -645,9 +735,100 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="63" x14ac:dyDescent="0.4">
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="44.4" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="42" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="44.4" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="44.4" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="84" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="105" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -662,8 +843,48 @@
     <hyperlink ref="A10" r:id="rId8" xr:uid="{D384F9A0-26A2-4408-9968-D0218DBCF23B}"/>
     <hyperlink ref="A11" r:id="rId9" xr:uid="{9F625D65-7BF6-4CD3-8B96-5BF6E533E694}"/>
     <hyperlink ref="A13" r:id="rId10" xr:uid="{AD99E3A2-C599-4B30-93D8-D66579AD285D}"/>
+    <hyperlink ref="A16" r:id="rId11" xr:uid="{A889B5A8-C160-4A86-93B6-B2C053026E19}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{D56CD892-76AA-48F1-BE21-908771E99A2A}"/>
+    <hyperlink ref="A20" r:id="rId13" xr:uid="{8098BBC8-8B07-42FE-B730-AD4D90889357}"/>
+    <hyperlink ref="A21" r:id="rId14" xr:uid="{F952E544-81F9-40A2-8D10-3D6C4FF3B022}"/>
+    <hyperlink ref="A22" r:id="rId15" xr:uid="{3B0CA622-224C-410F-B9BF-9F8418B9B17F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2251B660-D672-424C-A14A-EE57D04B6308}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="135.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" tooltip="Learn more about text retrieval system from ScienceDirect's AI-generated Topic Pages" display="https://www.sciencedirect.com/topics/computer-science/text-retrieval-system" xr:uid="{4C4695C3-C4AD-4460-AEC7-2970FD6DBFB7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>